<commit_message>
Drill using TLC and TLC+ formats
</commit_message>
<xml_diff>
--- a/PQ_Efficiency_Drills.xlsx
+++ b/PQ_Efficiency_Drills.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{92E08124-A9FD-4D50-B29B-AA58E7C53525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F931038-9639-40B2-85D1-B84D40D33C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Formats" sheetId="2" r:id="rId2"/>
-    <sheet name="Lists" sheetId="3" r:id="rId3"/>
+    <sheet name="PQ_Connection_Only" sheetId="1" r:id="rId1"/>
+    <sheet name="TLC4Graphics" sheetId="4" r:id="rId2"/>
+    <sheet name="Formats" sheetId="2" r:id="rId3"/>
+    <sheet name="Lists" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -84,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>FROM:</t>
   </si>
@@ -169,11 +170,44 @@
   <si>
     <t>Four</t>
   </si>
+  <si>
+    <t>26-Nov-2023</t>
+  </si>
+  <si>
+    <t>TLC Method for Graphs</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value1</t>
+  </si>
+  <si>
+    <t>Value2</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="mmm"/>
+  </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -362,7 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -656,7 +690,2256 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TLC4Graphics!$C$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TLC4Graphics!$B$8:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>mmm</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44958</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44986</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45047</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45078</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45108</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45139</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45170</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45231</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45261</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TLC4Graphics!$C$8:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9258-4874-A260-008778B07ADE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TLC4Graphics!$D$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>TLC4Graphics!$B$8:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>mmm</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>44927</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44958</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44986</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45017</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45047</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45078</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45108</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45139</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45170</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45231</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45261</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>TLC4Graphics!$D$8:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9258-4874-A260-008778B07ADE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="18648224"/>
+        <c:axId val="670261504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="18648224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="mmm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="670261504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="670261504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="18648224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.965966754155731E-2"/>
+          <c:y val="1.3888888888888888E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TLC4Graphics!$D$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TLC4Graphics!$B$25:$C$36</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Jul</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Aug</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sep</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Oct</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Nov</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Dec</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>First</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Second</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Third</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Fourth</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TLC4Graphics!$D$25:$D$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4927-4051-8AD1-FDD236F7E5F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TLC4Graphics!$E$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Value2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>TLC4Graphics!$B$25:$C$36</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="12"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>May</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Jun</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Jul</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Aug</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Sep</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Oct</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Nov</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Dec</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>First</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Second</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Third</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Fourth</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TLC4Graphics!$E$25:$E$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4927-4051-8AD1-FDD236F7E5F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2024282976"/>
+        <c:axId val="670259024"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2024282976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="670259024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="670259024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2024282976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.62655555555555553"/>
+          <c:y val="7.6691819772528397E-2"/>
+          <c:w val="0.35799999999999998"/>
+          <c:h val="7.6085958005249338E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{934502DF-14DE-F3AD-0B3D-BBE3063E02ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>41910</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>346710</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A15574D-B8F4-9C9A-6B12-D37F7E911BF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -784,7 +3067,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1091,8 +3374,8 @@
   </sheetPr>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1218,6 +3501,356 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B1DE03-72A2-4988-8A70-EFE02EFCBE7F}">
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" cm="1">
+        <f t="array" ref="B8:B19">DATE(2023,_xlfn.SEQUENCE(12,1,1),1)</f>
+        <v>44927</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <v>44958</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>44986</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
+        <v>45017</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>45047</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <v>45078</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="9">
+        <v>45108</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="9">
+        <v>45139</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="9">
+        <v>45170</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="9">
+        <v>45200</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="9">
+        <v>45231</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="9">
+        <v>45261</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="9" cm="1">
+        <f t="array" ref="C25:C36">DATE(2023,_xlfn.SEQUENCE(12,1,1),1)</f>
+        <v>44927</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="9">
+        <v>44958</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="9">
+        <v>44986</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="9">
+        <v>45017</v>
+      </c>
+      <c r="D28">
+        <v>4</v>
+      </c>
+      <c r="E28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="9">
+        <v>45047</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="9">
+        <v>45078</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="9">
+        <v>45108</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="9">
+        <v>45139</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="9">
+        <v>45170</v>
+      </c>
+      <c r="D33">
+        <v>9</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="9">
+        <v>45200</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="9">
+        <v>45231</v>
+      </c>
+      <c r="D35">
+        <v>11</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="9">
+        <v>45261</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E8867-A2D1-43A4-9ACC-7AB2760F7CD8}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -1255,7 +3888,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>25-Nov-2023</v>
+        <v>26-Nov-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1391,19 +4024,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1411,11 +4040,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1423,19 +4051,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1443,11 +4067,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1455,19 +4078,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1475,11 +4094,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1487,13 +4105,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>
@@ -1531,7 +4149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E13436D-CE0C-4639-B951-C1B98556791F}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -1566,7 +4184,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>25-Nov-2023</v>
+        <v>26-Nov-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Tried something Diramuid appeared to do
</commit_message>
<xml_diff>
--- a/PQ_Efficiency_Drills.xlsx
+++ b/PQ_Efficiency_Drills.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F931038-9639-40B2-85D1-B84D40D33C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5BD933-88CB-465F-B69E-FAC18AA02D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="PQ_Connection_Only" sheetId="1" r:id="rId1"/>
     <sheet name="TLC4Graphics" sheetId="4" r:id="rId2"/>
-    <sheet name="Formats" sheetId="2" r:id="rId3"/>
-    <sheet name="Lists" sheetId="3" r:id="rId4"/>
+    <sheet name="BYROWnoLambda" sheetId="5" r:id="rId3"/>
+    <sheet name="Formats" sheetId="2" r:id="rId4"/>
+    <sheet name="Lists" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="8" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -85,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>FROM:</t>
   </si>
@@ -200,13 +201,22 @@
   <si>
     <t>Fourth</t>
   </si>
+  <si>
+    <t>27-Nov-2023</t>
+  </si>
+  <si>
+    <t>BYROW No Lambda</t>
+  </si>
+  <si>
+    <t>I saw Diramuid use a BYROW and tried it with no lambda. I cannot find where that is supported.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="mmm"/>
+    <numFmt numFmtId="164" formatCode="mmm"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -396,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -3170,6 +3180,18 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A497FD9-964A-4B4C-9118-C4926BEE114C}" name="Table3" displayName="Table3" ref="B7:D17" totalsRowShown="0">
+  <autoFilter ref="B7:D17" xr:uid="{9A497FD9-964A-4B4C-9118-C4926BEE114C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DE449C1F-BBF5-42ED-8FFD-0965146DF2E8}" name="A"/>
+    <tableColumn id="2" xr3:uid="{C520C00D-D42B-4FF2-B458-6C7E7D4D5C81}" name="B"/>
+    <tableColumn id="3" xr3:uid="{C2577E6D-297F-4A01-AA3E-D08CFA509391}" name="C"/>
+  </tableColumns>
+  <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33EBBF0F-200B-49A7-BE86-E02A26DD1F32}" name="_tSample" displayName="_tSample" ref="B7:E13" totalsRowShown="0">
   <autoFilter ref="B7:E13" xr:uid="{33EBBF0F-200B-49A7-BE86-E02A26DD1F32}"/>
   <tableColumns count="4">
@@ -3504,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B1DE03-72A2-4988-8A70-EFE02EFCBE7F}">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3851,6 +3873,209 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5164F6D4-9D3D-447E-96AE-18A1919A99C8}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>44</v>
+      </c>
+      <c r="C8">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>60</v>
+      </c>
+      <c r="F8" cm="1">
+        <f t="array" ref="F8:F17">_xlfn.BYROW(Table3[],_xlfn.LAMBDA(_xlpm.x,SUM(_xlpm.x)))</f>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>18</v>
+      </c>
+      <c r="F9">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>66</v>
+      </c>
+      <c r="F10">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>51</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>81</v>
+      </c>
+      <c r="F11">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>39</v>
+      </c>
+      <c r="D12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>42</v>
+      </c>
+      <c r="C13">
+        <v>98</v>
+      </c>
+      <c r="D13">
+        <v>51</v>
+      </c>
+      <c r="F13">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>96</v>
+      </c>
+      <c r="C14">
+        <v>88</v>
+      </c>
+      <c r="D14">
+        <v>91</v>
+      </c>
+      <c r="F14">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>96</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+      <c r="F15">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>57</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>25</v>
+      </c>
+      <c r="F16">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>52</v>
+      </c>
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>75</v>
+      </c>
+      <c r="F17">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E8867-A2D1-43A4-9ACC-7AB2760F7CD8}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -3888,7 +4113,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>26-Nov-2023</v>
+        <v>27-Nov-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -4149,7 +4374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E13436D-CE0C-4639-B951-C1B98556791F}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -4184,7 +4409,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>26-Nov-2023</v>
+        <v>27-Nov-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Trying other BYROW alternatives
</commit_message>
<xml_diff>
--- a/PQ_Efficiency_Drills.xlsx
+++ b/PQ_Efficiency_Drills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5BD933-88CB-465F-B69E-FAC18AA02D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB661E1C-03DB-48AF-9DE9-4FDFC29D27D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -24,8 +24,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3077,7 +3078,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -3874,15 +3875,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5164F6D4-9D3D-447E-96AE-18A1919A99C8}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3891,7 +3892,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3900,7 +3901,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -3909,12 +3910,12 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>8</v>
       </c>
@@ -3925,7 +3926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>44</v>
       </c>
@@ -3939,8 +3940,12 @@
         <f t="array" ref="F8:F17">_xlfn.BYROW(Table3[],_xlfn.LAMBDA(_xlpm.x,SUM(_xlpm.x)))</f>
         <v>133</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8" t="e" cm="1">
+        <f t="array" ref="H8">_xlfn.BYROW(Table3[],SUM)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>80</v>
       </c>
@@ -3954,7 +3959,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>80</v>
       </c>
@@ -3968,7 +3973,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>51</v>
       </c>
@@ -3982,7 +3987,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>57</v>
       </c>
@@ -3996,7 +4001,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>42</v>
       </c>
@@ -4010,7 +4015,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>96</v>
       </c>
@@ -4024,7 +4029,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>96</v>
       </c>
@@ -4038,7 +4043,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>57</v>
       </c>
@@ -4113,7 +4118,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>27-Nov-2023</v>
+        <v>29-Nov-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -4409,7 +4414,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>27-Nov-2023</v>
+        <v>29-Nov-2023</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>